<commit_message>
add test suite collection for login, register, and visit
</commit_message>
<xml_diff>
--- a/Data Files/01_Login Data.xlsx
+++ b/Data Files/01_Login Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\git\Automation-openRMS\Data Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{763B8BCA-C9A5-4BB6-9B3C-1925213A3CD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{428B336F-1C73-41BB-81A5-16EB7DF1BB3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="380" windowWidth="14400" windowHeight="7270" xr2:uid="{002CBD15-2C30-496C-85A2-1A54428D15E2}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{002CBD15-2C30-496C-85A2-1A54428D15E2}"/>
   </bookViews>
   <sheets>
     <sheet name="Location" sheetId="1" r:id="rId1"/>
@@ -19,17 +19,6 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>

</xml_diff>